<commit_message>
Figure changes for resubmission #2
</commit_message>
<xml_diff>
--- a/Table 2 - Diagnostic Pigments/Table2-ChloropigmentTable.xlsx
+++ b/Table 2 - Diagnostic Pigments/Table2-ChloropigmentTable.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25317"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="20" yWindow="0" windowWidth="24640" windowHeight="13940" tabRatio="500"/>
+    <workbookView xWindow="13480" yWindow="0" windowWidth="37560" windowHeight="26000" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="37">
   <si>
     <t xml:space="preserve">Diagnostic Pigments </t>
   </si>
@@ -75,22 +75,13 @@
     <t>picoplankton</t>
   </si>
   <si>
-    <t>Cyanobacteria and prochlorophytes</t>
-  </si>
-  <si>
     <t>Diatoms</t>
   </si>
   <si>
     <t>Dinoflagellates</t>
   </si>
   <si>
-    <t>Chromophytes and nanoflagellates</t>
-  </si>
-  <si>
     <t>Cryptophytes</t>
-  </si>
-  <si>
-    <t>Green flagellates and prochlorophytes</t>
   </si>
   <si>
     <t>Estimation formula</t>
@@ -138,6 +129,18 @@
       </rPr>
       <t>b</t>
     </r>
+  </si>
+  <si>
+    <t>Green algae (green flagellates and prochlorophytes)</t>
+  </si>
+  <si>
+    <t>Prokaryotes (cyanobacteria and prochlorophytes)</t>
+  </si>
+  <si>
+    <t>Pelagophytes (chromophytes and nanoflagellates)</t>
+  </si>
+  <si>
+    <t>Prymensiophytes (chromophytes and nanoflagellates)</t>
   </si>
 </sst>
 </file>
@@ -692,12 +695,12 @@
   <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="27.6640625" customWidth="1"/>
+    <col min="1" max="1" width="38.5" customWidth="1"/>
     <col min="2" max="2" width="21.1640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.83203125" customWidth="1"/>
     <col min="5" max="5" width="11.5" customWidth="1"/>
@@ -705,7 +708,7 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -714,7 +717,7 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="4" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>0</v>
@@ -723,15 +726,15 @@
         <v>7</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>1</v>
@@ -740,7 +743,7 @@
         <v>8</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>15</v>
@@ -748,7 +751,7 @@
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>2</v>
@@ -757,7 +760,7 @@
         <v>9</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>15</v>
@@ -765,7 +768,7 @@
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="2" t="s">
-        <v>21</v>
+        <v>36</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>5</v>
@@ -774,7 +777,7 @@
         <v>10</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>16</v>
@@ -782,7 +785,7 @@
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="2" t="s">
-        <v>21</v>
+        <v>35</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>6</v>
@@ -791,7 +794,7 @@
         <v>11</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>16</v>
@@ -799,7 +802,7 @@
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>3</v>
@@ -808,7 +811,7 @@
         <v>14</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>16</v>
@@ -816,16 +819,16 @@
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="2" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>12</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>17</v>
@@ -833,7 +836,7 @@
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="3" t="s">
-        <v>18</v>
+        <v>34</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>4</v>
@@ -842,7 +845,7 @@
         <v>13</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="E9" s="3" t="s">
         <v>17</v>

</xml_diff>

<commit_message>
Changed PFT descriptions in Table 2 (e.g. coccolithophores)
</commit_message>
<xml_diff>
--- a/Table 2 - Diagnostic Pigments/Table2-ChloropigmentTable.xlsx
+++ b/Table 2 - Diagnostic Pigments/Table2-ChloropigmentTable.xlsx
@@ -140,7 +140,7 @@
     <t>Pelagophytes (chromophytes and nanoflagellates)</t>
   </si>
   <si>
-    <t>Prymensiophytes (chromophytes and nanoflagellates)</t>
+    <t>Prymensiophytes (coccolithophores)</t>
   </si>
 </sst>
 </file>
@@ -695,7 +695,7 @@
   <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>